<commit_message>
week 9 tutorial attempt, q1 half way done
</commit_message>
<xml_diff>
--- a/Assignment1/finalk.xlsx
+++ b/Assignment1/finalk.xlsx
@@ -443,7 +443,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
@@ -451,7 +451,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -459,7 +459,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -467,7 +467,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
@@ -475,7 +475,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -483,7 +483,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -491,7 +491,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9">
@@ -499,7 +499,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -507,7 +507,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11">
@@ -515,7 +515,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12">
@@ -523,7 +523,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13">
@@ -531,7 +531,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14">
@@ -555,7 +555,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -563,7 +563,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18">
@@ -571,7 +571,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19">
@@ -579,7 +579,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20">
@@ -587,7 +587,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21">
@@ -595,7 +595,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
@@ -603,7 +603,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23">
@@ -611,7 +611,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24">
@@ -627,7 +627,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
@@ -635,7 +635,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27">
@@ -651,7 +651,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29">
@@ -659,7 +659,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
@@ -675,7 +675,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32">
@@ -683,7 +683,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
@@ -691,7 +691,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34">
@@ -699,7 +699,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35">
@@ -707,7 +707,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36">
@@ -715,7 +715,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37">
@@ -723,7 +723,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38">
@@ -731,7 +731,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39">
@@ -739,7 +739,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40">
@@ -747,7 +747,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41">
@@ -755,7 +755,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42">
@@ -763,7 +763,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43">
@@ -771,7 +771,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="44">
@@ -787,7 +787,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46">
@@ -795,7 +795,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47">
@@ -811,7 +811,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49">
@@ -819,7 +819,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50">
@@ -827,7 +827,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51">
@@ -835,7 +835,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52">
@@ -851,7 +851,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="54">
@@ -859,7 +859,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55">
@@ -867,7 +867,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56">
@@ -883,7 +883,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="58">
@@ -891,7 +891,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="59">
@@ -899,7 +899,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="60">
@@ -907,7 +907,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61">
@@ -915,7 +915,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62">
@@ -923,7 +923,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63">
@@ -939,7 +939,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="65">
@@ -963,7 +963,7 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68">
@@ -979,7 +979,7 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70">
@@ -987,7 +987,7 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="71">
@@ -995,7 +995,7 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="72">
@@ -1003,7 +1003,7 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73">
@@ -1011,7 +1011,7 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74">
@@ -1027,7 +1027,7 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="76">
@@ -1035,7 +1035,7 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77">
@@ -1043,7 +1043,7 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="78">
@@ -1059,7 +1059,7 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="80">
@@ -1067,7 +1067,7 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="81">
@@ -1083,7 +1083,7 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="83">
@@ -1091,7 +1091,7 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84">
@@ -1099,7 +1099,7 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="85">
@@ -1107,7 +1107,7 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86">
@@ -1115,7 +1115,7 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="87">
@@ -1123,7 +1123,7 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="88">
@@ -1131,7 +1131,7 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="89">
@@ -1139,7 +1139,7 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="90">
@@ -1147,7 +1147,7 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="91">
@@ -1155,7 +1155,7 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92">
@@ -1163,7 +1163,7 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93">
@@ -1171,7 +1171,7 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="94">
@@ -1179,7 +1179,7 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="95">
@@ -1187,7 +1187,7 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="96">
@@ -1195,7 +1195,7 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="97">
@@ -1203,7 +1203,7 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="98">
@@ -1211,7 +1211,7 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="99">
@@ -1219,7 +1219,7 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="100">
@@ -1227,7 +1227,7 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>